<commit_message>
Added formatted clean data and a functional Streamlit app draft
</commit_message>
<xml_diff>
--- a/data/mapping_tables.xlsx
+++ b/data/mapping_tables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_maerskbroker_com/Documents/Documents/M scraper/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="385" documentId="8_{E82970A2-BBD4-4F32-BE27-31237F44A44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F82863B-A3F2-46E9-9085-CD0C2B051FD7}"/>
+  <xr:revisionPtr revIDLastSave="637" documentId="8_{E82970A2-BBD4-4F32-BE27-31237F44A44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68B89CBA-9803-41DF-9320-A846EF582A4E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BAC1D2B-409C-4654-934D-3906D9663A7C}"/>
   </bookViews>
@@ -57,10 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="127">
-  <si>
-    <t>status</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="183">
   <si>
     <t>status_en</t>
   </si>
@@ -438,13 +435,185 @@
   </si>
   <si>
     <t>Ny Ellebjerg</t>
+  </si>
+  <si>
+    <t>Passagerer til og fra Lufthavnen skal skifte tog på Femøren</t>
+  </si>
+  <si>
+    <t>Vores sporarbejde er 15-20 min. forsinket her til morgen</t>
+  </si>
+  <si>
+    <t>Bemærk vedligehold! Fra kl. 00:00-05:00 er M1/M2 lukket. Metrobusser indsættes ml. Vanløse - CPH Lufthavn &amp; Vanløse - Vestamager. Metrobusserne kører hvert 20. minut</t>
+  </si>
+  <si>
+    <t>Vi er ramt af forsinkelser. Vi kører snart normalt igen</t>
+  </si>
+  <si>
+    <t>Vi er ramt af forsinkelser. Vi kører snart normalt!</t>
+  </si>
+  <si>
+    <t>Alle tog holder stille grundet tekniske problemer. Intet tidsestimat for genoptaget drift.</t>
+  </si>
+  <si>
+    <t>Passagerer der skal til Orientkaj skal skifte tog på Østerport.</t>
+  </si>
+  <si>
+    <t>PA: (DK/UK): Passagerer der skal til Orientkaj skal skifte tog på Østerport. Forvent længere rejsetid i begge spor.</t>
+  </si>
+  <si>
+    <t>Passager til Orientkaj, skal skifte tog på Østerport.</t>
+  </si>
+  <si>
+    <t>I øjeblikket er der ingen drift i spor 2 mellem Østerport og KH men der er normal drift i spor 1. M4: Ingen drift mellem Østerport og Nordhavn, brug evt. S-tog i stedet for.</t>
+  </si>
+  <si>
+    <t>I øjeblikket er der ingen drift i spor 2 mellem Østerport og KH men der er normal drift i spor 1. M4: Ingen drift mellem Østerport og Nordhavn</t>
+  </si>
+  <si>
+    <t>Der i øjeblikket ingen drift i spor 2 men normal drift i spor 1. ingen togdrift på M4 linjen</t>
+  </si>
+  <si>
+    <t>M3: Der i øjeblikket ingen drift i spor 2 men normal drift i spor 1. M4: Ingen togdrift</t>
+  </si>
+  <si>
+    <t>Alle tog holder i øjeblikket stille grundet tekniske problemer ved Østerport</t>
+  </si>
+  <si>
+    <t>Ingen drift Christianshavn-Lufthavnen.</t>
+  </si>
+  <si>
+    <t>Ingen drift Vanløse-Frederiksberg og Christianshavn-Lufthavnen.</t>
+  </si>
+  <si>
+    <t>Ingen tog drift, 10-15 min forsinkelse.</t>
+  </si>
+  <si>
+    <t>Flere tog holder stille, problemer ved Femøren og Vanløse.</t>
+  </si>
+  <si>
+    <t>Ingen tog drift, Vanløse-Frederiksberg. 8 min forsinkelse.</t>
+  </si>
+  <si>
+    <t>Ingen tog drift Vanløse til Frederiksberg.</t>
+  </si>
+  <si>
+    <t>Vi kan i øjeblikket ikke benytte spor 1 på Christianshavn, tag toget i spor 2 til Kongens Nytorv og skift til tog mod Vestamager eller Lufthavnen derfra</t>
+  </si>
+  <si>
+    <t>Vi holder stille i begge spor grundet tekniske problemer med et tog på Københavns Hovedbanegård. Intet tidsestimat for genoptaget drift.</t>
+  </si>
+  <si>
+    <t>Ingen tog standser på Aksel Møllers Have grundet en brandalarm på stationen.</t>
+  </si>
+  <si>
+    <t>Forsinkelser til/fra Vestamager grundet tekniske problemer ved Sundby.</t>
+  </si>
+  <si>
+    <t>Ingen tog stopper på Fasanvej grundet en brandalarm.</t>
+  </si>
+  <si>
+    <t>Ingen tog standser på Vibenhus Runddel, det skyldes en brandalarm</t>
+  </si>
+  <si>
+    <t>Flere tog holder stille, 5-8 min forsinkelse.</t>
+  </si>
+  <si>
+    <t>M4: Ingen togdrift mellem Østerport og Orientkaj i begge retninger før kl. 02:50, grundet tekniske problemer.</t>
+  </si>
+  <si>
+    <t>M1_All, M2_All</t>
+  </si>
+  <si>
+    <t>Nordhavn, Orientkaj</t>
+  </si>
+  <si>
+    <t>M4_All</t>
+  </si>
+  <si>
+    <t>Nordhavn, Østerport, Marmorkirken, Kongens Nytorv, Gammel Strand, Rådhuspladsen, Københavns Hovedbanegård</t>
+  </si>
+  <si>
+    <t>Amagerbro, Lergravsparken, Øresund, Amager Strand, Femøren, Kastrup, CPH Lufthavn</t>
+  </si>
+  <si>
+    <t>Amagerbro, Lergravsparken, Øresund, Amager Strand, Femøren, Kastrup, CPH Lufthavn, Vanløse, Flintholm, Lindevang, Fasanvej</t>
+  </si>
+  <si>
+    <t>Femøren, Vanløse</t>
+  </si>
+  <si>
+    <t>Vanløse, Flintholm, Lindevang, Fasanvej</t>
+  </si>
+  <si>
+    <t>Amagerbro, Lergravsparken, Øresund, Amager Strand, Femøren, Kastrup, CPH Lufthavn, Islands Brygge, DR Byen, Sundby, Bella Center, Ørestad, Vestamager</t>
+  </si>
+  <si>
+    <t>Islands Brygge, DR Byen, Sundby, Bella Center, Ørestad, Vestamager</t>
+  </si>
+  <si>
+    <t>Vibenhus Runddel</t>
+  </si>
+  <si>
+    <t>Til/fra CPH Lufthavnen skal du skifte tog på Femøren. Længere rejsetid må forventes.</t>
+  </si>
+  <si>
+    <t>Alle tog holder stille, det skyldes tog med fejlramt dør på Christianshavn</t>
+  </si>
+  <si>
+    <t>Flere tog holder stille, det skyldes problemer med en togdør på Christianshavn.
+Til/fra CPH Lufthavnen, skal du skifte tog på Femøren</t>
+  </si>
+  <si>
+    <t>Vi stopper ikke på Amager Strand spor1.</t>
+  </si>
+  <si>
+    <t>Togskifte på Øresund til og fra Lufthavnen.</t>
+  </si>
+  <si>
+    <t>Tog skifte til og fra Lufthavnen.</t>
+  </si>
+  <si>
+    <t>Vores sporarbejde er ca. 10 min. forsinket</t>
+  </si>
+  <si>
+    <t>Vores sporarbejde er ca. 25 min. forsinket</t>
+  </si>
+  <si>
+    <t>Ingen tog drift Vanløse-Nørreport.</t>
+  </si>
+  <si>
+    <t>10 min forsinkelse på hele banen.</t>
+  </si>
+  <si>
+    <t>Ingen tog drift Vanløse-Frederiksberg.</t>
+  </si>
+  <si>
+    <t>Øresund, Femøren, Kastrup, CPH Lufthavn</t>
+  </si>
+  <si>
+    <t>Vanløse, Flintholm, Lindevang, Fasanvej, Frederiksberg</t>
+  </si>
+  <si>
+    <t>Vanløse, Flintholm, Lindevang, Fasanvej, Frederiksberg, Forum, Nørreport</t>
+  </si>
+  <si>
+    <t>Nattens sporarbejde er forsinket. Vi forventer at køre igen i spor 2 kl. 5:30. Benyt spor 1 i stedet.</t>
+  </si>
+  <si>
+    <t>Vi stopper ikke på Amager Strand spor 1.</t>
+  </si>
+  <si>
+    <t>status_dk</t>
+  </si>
+  <si>
+    <t>Lukket frem til kl. 05:00 pga. sporarbejde. Metrobusser kører hvert 20. minut. Se afgangstider på rejseplanen.dk</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,12 +626,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -555,10 +718,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C314E41B-CB9C-4666-8112-1C776CCF8BCF}" name="Table2" displayName="Table2" ref="A1:I18" totalsRowShown="0">
-  <autoFilter ref="A1:I18" xr:uid="{C314E41B-CB9C-4666-8112-1C776CCF8BCF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C314E41B-CB9C-4666-8112-1C776CCF8BCF}" name="Table2" displayName="Table2" ref="A1:I60" totalsRowShown="0">
+  <autoFilter ref="A1:I60" xr:uid="{C314E41B-CB9C-4666-8112-1C776CCF8BCF}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A2B24526-B093-4F61-8528-751DBACD919A}" name="status" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{A2B24526-B093-4F61-8528-751DBACD919A}" name="status_dk" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{AF80EE63-ECB6-42AC-8C94-7AE1E4203C14}" name="status_en" dataDxfId="9"/>
     <tableColumn id="10" xr3:uid="{CE0DD46B-3B95-4543-9C5D-90ABA92B907A}" name="reason" dataDxfId="8"/>
     <tableColumn id="7" xr3:uid="{E72E3A80-9EBE-4D70-8250-23D610E05193}" name="closed_for_maintenance" dataDxfId="7"/>
@@ -916,10 +1079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E59BAE-EAED-4611-9ECD-D2146E9DBD95}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,42 +1100,42 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>181</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>23</v>
       </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
       <c r="H1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" s="4">
         <v>0</v>
@@ -990,18 +1153,18 @@
         <v>0</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
@@ -1012,13 +1175,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1031,13 +1194,13 @@
     </row>
     <row r="5" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1055,18 +1218,18 @@
         <v>0</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
@@ -1084,18 +1247,18 @@
         <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
@@ -1113,18 +1276,18 @@
         <v>0</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -1145,129 +1308,129 @@
     </row>
     <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="4">
         <v>0</v>
@@ -1285,18 +1448,18 @@
         <v>0</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
@@ -1317,72 +1480,72 @@
     </row>
     <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>1</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>1</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="D17" s="4">
         <v>0</v>
       </c>
@@ -1398,44 +1561,1241 @@
       <c r="H17" s="4">
         <v>0</v>
       </c>
-      <c r="I17" s="3" t="s">
-        <v>56</v>
-      </c>
+      <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="4">
+        <v>0</v>
+      </c>
+      <c r="H18" s="4">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0</v>
+      </c>
+      <c r="G19" s="4">
+        <v>0</v>
+      </c>
+      <c r="H19" s="4">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4">
-        <v>1</v>
-      </c>
-      <c r="F18" s="4">
-        <v>0</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0</v>
-      </c>
-      <c r="H18" s="4">
-        <v>1</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0</v>
+      </c>
+      <c r="G20" s="4">
+        <v>0</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="4">
+        <v>1</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0</v>
+      </c>
+      <c r="G21" s="4">
+        <v>0</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0</v>
+      </c>
+      <c r="G22" s="4">
+        <v>0</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="4">
+        <v>1</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
+      <c r="F25" s="4">
+        <v>0</v>
+      </c>
+      <c r="G25" s="4">
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
+        <v>1</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D26" s="4">
+        <v>0</v>
+      </c>
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
+      <c r="F26" s="4">
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4">
+        <v>1</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="4">
+        <v>0</v>
+      </c>
+      <c r="E27" s="4">
+        <v>1</v>
+      </c>
+      <c r="F27" s="4">
+        <v>0</v>
+      </c>
+      <c r="G27" s="4">
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4">
+        <v>1</v>
+      </c>
+      <c r="F28" s="4">
+        <v>1</v>
+      </c>
+      <c r="G28" s="4">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+      <c r="E29" s="4">
+        <v>1</v>
+      </c>
+      <c r="F29" s="4">
+        <v>1</v>
+      </c>
+      <c r="G29" s="4">
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="4">
+        <v>0</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1</v>
+      </c>
+      <c r="F30" s="4">
+        <v>1</v>
+      </c>
+      <c r="G30" s="4">
+        <v>0</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="4">
+        <v>0</v>
+      </c>
+      <c r="E31" s="4">
+        <v>1</v>
+      </c>
+      <c r="F31" s="4">
+        <v>1</v>
+      </c>
+      <c r="G31" s="4">
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>1</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+      <c r="E33" s="4">
+        <v>0</v>
+      </c>
+      <c r="F33" s="4">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4">
+        <v>0</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="4">
+        <v>0</v>
+      </c>
+      <c r="E34" s="4">
+        <v>0</v>
+      </c>
+      <c r="F34" s="4">
+        <v>1</v>
+      </c>
+      <c r="G34" s="4">
+        <v>0</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D35" s="4">
+        <v>0</v>
+      </c>
+      <c r="E35" s="4">
+        <v>1</v>
+      </c>
+      <c r="F35" s="4">
+        <v>1</v>
+      </c>
+      <c r="G35" s="4">
+        <v>0</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="4">
+        <v>0</v>
+      </c>
+      <c r="E36" s="4">
+        <v>1</v>
+      </c>
+      <c r="F36" s="4">
+        <v>1</v>
+      </c>
+      <c r="G36" s="4">
+        <v>0</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37" s="4">
+        <v>0</v>
+      </c>
+      <c r="E37" s="4">
+        <v>1</v>
+      </c>
+      <c r="F37" s="4">
+        <v>1</v>
+      </c>
+      <c r="G37" s="4">
+        <v>0</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" s="4">
+        <v>0</v>
+      </c>
+      <c r="E38" s="4">
+        <v>1</v>
+      </c>
+      <c r="F38" s="4">
+        <v>1</v>
+      </c>
+      <c r="G38" s="4">
+        <v>0</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="144" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="4">
+        <v>0</v>
+      </c>
+      <c r="E39" s="4">
+        <v>1</v>
+      </c>
+      <c r="F39" s="4">
+        <v>1</v>
+      </c>
+      <c r="G39" s="4">
+        <v>0</v>
+      </c>
+      <c r="H39" s="4">
+        <v>1</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="4">
+        <v>0</v>
+      </c>
+      <c r="E40" s="4">
+        <v>1</v>
+      </c>
+      <c r="F40" s="4">
+        <v>1</v>
+      </c>
+      <c r="G40" s="4">
+        <v>0</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="4">
+        <v>0</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0</v>
+      </c>
+      <c r="F41" s="4">
+        <v>0</v>
+      </c>
+      <c r="G41" s="4">
+        <v>1</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+      <c r="E42" s="4">
+        <v>1</v>
+      </c>
+      <c r="F42" s="4">
+        <v>0</v>
+      </c>
+      <c r="G42" s="4">
+        <v>0</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D43" s="4">
+        <v>0</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0</v>
+      </c>
+      <c r="F43" s="4">
+        <v>0</v>
+      </c>
+      <c r="G43" s="4">
+        <v>1</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0</v>
+      </c>
+      <c r="E44" s="4">
+        <v>0</v>
+      </c>
+      <c r="F44" s="4">
+        <v>0</v>
+      </c>
+      <c r="G44" s="4">
+        <v>1</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+      <c r="E45" s="4">
+        <v>1</v>
+      </c>
+      <c r="F45" s="4">
+        <v>0</v>
+      </c>
+      <c r="G45" s="4">
+        <v>0</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+      <c r="E46" s="4">
+        <v>1</v>
+      </c>
+      <c r="F46" s="4">
+        <v>1</v>
+      </c>
+      <c r="G46" s="4">
+        <v>0</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
+      </c>
+      <c r="E47" s="4">
+        <v>1</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0</v>
+      </c>
+      <c r="G47" s="4">
+        <v>0</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="4">
+        <v>0</v>
+      </c>
+      <c r="E48" s="4">
+        <v>1</v>
+      </c>
+      <c r="F48" s="4">
+        <v>1</v>
+      </c>
+      <c r="G48" s="4">
+        <v>0</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="4">
+        <v>0</v>
+      </c>
+      <c r="E49" s="4">
+        <v>1</v>
+      </c>
+      <c r="F49" s="4">
+        <v>0</v>
+      </c>
+      <c r="G49" s="4">
+        <v>0</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" s="4">
+        <v>0</v>
+      </c>
+      <c r="E50" s="4">
+        <v>0</v>
+      </c>
+      <c r="F50" s="4">
+        <v>0</v>
+      </c>
+      <c r="G50" s="4">
+        <v>1</v>
+      </c>
+      <c r="H50" s="4">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="4">
+        <v>0</v>
+      </c>
+      <c r="E51" s="4">
+        <v>1</v>
+      </c>
+      <c r="F51" s="4">
+        <v>0</v>
+      </c>
+      <c r="G51" s="4">
+        <v>0</v>
+      </c>
+      <c r="H51" s="4">
+        <v>1</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D52" s="4">
+        <v>0</v>
+      </c>
+      <c r="E52" s="4">
+        <v>1</v>
+      </c>
+      <c r="F52" s="4">
+        <v>0</v>
+      </c>
+      <c r="G52" s="4">
+        <v>0</v>
+      </c>
+      <c r="H52" s="4">
+        <v>1</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D53" s="4">
+        <v>1</v>
+      </c>
+      <c r="E53" s="4">
+        <v>1</v>
+      </c>
+      <c r="F53" s="4">
+        <v>1</v>
+      </c>
+      <c r="G53" s="4">
+        <v>0</v>
+      </c>
+      <c r="H53" s="4">
+        <v>0</v>
+      </c>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D54" s="4">
+        <v>1</v>
+      </c>
+      <c r="E54" s="4">
+        <v>1</v>
+      </c>
+      <c r="F54" s="4">
+        <v>1</v>
+      </c>
+      <c r="G54" s="4">
+        <v>0</v>
+      </c>
+      <c r="H54" s="4">
+        <v>0</v>
+      </c>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D55" s="4">
+        <v>0</v>
+      </c>
+      <c r="E55" s="4">
+        <v>0</v>
+      </c>
+      <c r="F55" s="4">
+        <v>1</v>
+      </c>
+      <c r="G55" s="4">
+        <v>0</v>
+      </c>
+      <c r="H55" s="4">
+        <v>0</v>
+      </c>
+      <c r="I55" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0</v>
+      </c>
+      <c r="E56" s="4">
+        <v>1</v>
+      </c>
+      <c r="F56" s="4">
+        <v>0</v>
+      </c>
+      <c r="G56" s="4">
+        <v>0</v>
+      </c>
+      <c r="H56" s="4">
+        <v>0</v>
+      </c>
+      <c r="I56" s="3"/>
+    </row>
+    <row r="57" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0</v>
+      </c>
+      <c r="E57" s="4">
+        <v>0</v>
+      </c>
+      <c r="F57" s="4">
+        <v>1</v>
+      </c>
+      <c r="G57" s="4">
+        <v>0</v>
+      </c>
+      <c r="H57" s="4">
+        <v>0</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" s="4">
+        <v>1</v>
+      </c>
+      <c r="E58" s="4">
+        <v>1</v>
+      </c>
+      <c r="F58" s="4">
+        <v>0</v>
+      </c>
+      <c r="G58" s="4">
+        <v>0</v>
+      </c>
+      <c r="H58" s="4">
+        <v>0</v>
+      </c>
+      <c r="I58" s="3"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D59" s="4">
+        <v>0</v>
+      </c>
+      <c r="E59" s="4">
+        <v>0</v>
+      </c>
+      <c r="F59" s="4">
+        <v>0</v>
+      </c>
+      <c r="G59" s="4">
+        <v>1</v>
+      </c>
+      <c r="H59" s="4">
+        <v>0</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D60" s="4">
+        <v>1</v>
+      </c>
+      <c r="E60" s="4">
+        <v>0</v>
+      </c>
+      <c r="F60" s="4">
+        <v>0</v>
+      </c>
+      <c r="G60" s="4">
+        <v>0</v>
+      </c>
+      <c r="H60" s="4">
+        <v>0</v>
+      </c>
+      <c r="I60" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1458,59 +2818,59 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
         <v>113</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>114</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>115</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>116</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>117</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>118</v>
-      </c>
-      <c r="G1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
       </c>
       <c r="D2">
         <v>2019</v>
       </c>
       <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>62</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
         <v>64</v>
-      </c>
-      <c r="B3" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
       </c>
       <c r="D3">
         <v>2007</v>
@@ -1522,18 +2882,18 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <v>2002</v>
@@ -1545,18 +2905,18 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5">
         <v>2002</v>
@@ -1568,18 +2928,18 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6">
         <v>2003</v>
@@ -1591,18 +2951,18 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7">
         <v>2003</v>
@@ -1614,18 +2974,18 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8">
         <v>2002</v>
@@ -1634,44 +2994,44 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D9">
         <v>2019</v>
       </c>
       <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>62</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10">
         <v>2003</v>
@@ -1683,18 +3043,18 @@
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11">
         <v>2003</v>
@@ -1706,18 +3066,18 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12">
         <v>2007</v>
@@ -1729,18 +3089,18 @@
         <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13">
         <v>2004</v>
@@ -1752,18 +3112,18 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14">
         <v>2004</v>
@@ -1775,18 +3135,18 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15">
         <v>2003</v>
@@ -1798,18 +3158,18 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16">
         <v>2003</v>
@@ -1821,18 +3181,18 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17">
         <v>2003</v>
@@ -1841,21 +3201,21 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D18">
         <v>2003</v>
@@ -1864,21 +3224,21 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D19">
         <v>2003</v>
@@ -1887,90 +3247,90 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20">
         <v>2019</v>
       </c>
       <c r="E20" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>62</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D21">
         <v>2019</v>
       </c>
       <c r="E21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
         <v>62</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22">
         <v>2019</v>
       </c>
       <c r="E22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>62</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D23">
         <v>2002</v>
@@ -1982,18 +3342,18 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D24">
         <v>2007</v>
@@ -2005,64 +3365,64 @@
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D25">
         <v>2019</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26">
         <v>2019</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27">
         <v>2002</v>
@@ -2074,18 +3434,18 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D28">
         <v>2002</v>
@@ -2097,18 +3457,18 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D29">
         <v>2002</v>
@@ -2120,18 +3480,18 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D30">
         <v>2002</v>
@@ -2143,18 +3503,18 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31">
         <v>2002</v>
@@ -2166,18 +3526,18 @@
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D32">
         <v>2003</v>
@@ -2189,18 +3549,18 @@
         <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33">
         <v>2003</v>
@@ -2212,18 +3572,18 @@
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34">
         <v>2007</v>
@@ -2235,133 +3595,133 @@
         <v>4</v>
       </c>
       <c r="G34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D35">
         <v>2019</v>
       </c>
       <c r="E35" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
         <v>62</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36">
         <v>2019</v>
       </c>
       <c r="E36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
         <v>62</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D37">
         <v>2020</v>
       </c>
       <c r="E37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F37">
         <v>2</v>
       </c>
       <c r="G37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D38">
         <v>2019</v>
       </c>
       <c r="E38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F38">
         <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B39" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39">
         <v>2019</v>
       </c>
       <c r="E39" t="s">
+        <v>61</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
         <v>62</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40">
         <v>2002</v>
@@ -2373,18 +3733,18 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41">
         <v>2002</v>
@@ -2396,64 +3756,64 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42">
         <v>2019</v>
       </c>
       <c r="E42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
         <v>62</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D43">
         <v>2020</v>
       </c>
       <c r="E43" t="s">
+        <v>61</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
         <v>62</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D44">
         <v>2002</v>
@@ -2465,18 +3825,18 @@
         <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D45">
         <v>2007</v>
@@ -2488,156 +3848,156 @@
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D46">
         <v>2019</v>
       </c>
       <c r="E46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B47" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D47">
         <v>2019</v>
       </c>
       <c r="E47" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48">
         <v>2019</v>
       </c>
       <c r="E48" t="s">
+        <v>61</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48" t="s">
         <v>62</v>
-      </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49">
         <v>2019</v>
       </c>
       <c r="E49" t="s">
+        <v>61</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49" t="s">
         <v>62</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D50">
         <v>2019</v>
       </c>
       <c r="E50" t="s">
+        <v>61</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50" t="s">
         <v>62</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D51">
         <v>2019</v>
       </c>
       <c r="E51" t="s">
+        <v>61</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
         <v>62</v>
-      </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D52">
         <v>2002</v>
@@ -2649,41 +4009,41 @@
         <v>3</v>
       </c>
       <c r="G52" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D53">
         <v>2019</v>
       </c>
       <c r="E53" t="s">
+        <v>61</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53" t="s">
         <v>62</v>
-      </c>
-      <c r="F53">
-        <v>1</v>
-      </c>
-      <c r="G53" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D54">
         <v>2003</v>
@@ -2695,18 +4055,18 @@
         <v>2</v>
       </c>
       <c r="G54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C55" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D55">
         <v>2003</v>
@@ -2718,18 +4078,18 @@
         <v>2</v>
       </c>
       <c r="G55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D56">
         <v>2002</v>
@@ -2741,109 +4101,109 @@
         <v>3</v>
       </c>
       <c r="G56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D57">
         <v>2019</v>
       </c>
       <c r="E57" t="s">
+        <v>61</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57" t="s">
         <v>62</v>
-      </c>
-      <c r="F57">
-        <v>1</v>
-      </c>
-      <c r="G57" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B58" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D58">
         <v>2024</v>
       </c>
       <c r="G58" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B59" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D59">
         <v>2024</v>
       </c>
       <c r="G59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B60" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C60" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D60">
         <v>2024</v>
       </c>
       <c r="G60" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C61" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D61">
         <v>2024</v>
       </c>
       <c r="G61" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B62" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D62">
         <v>2024</v>
@@ -2873,10 +4233,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2884,7 +4244,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2892,7 +4252,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2900,7 +4260,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2908,7 +4268,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2916,7 +4276,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2924,7 +4284,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2932,7 +4292,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2940,7 +4300,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2948,7 +4308,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -2956,7 +4316,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2964,7 +4324,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2972,7 +4332,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2980,7 +4340,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2988,7 +4348,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -2996,7 +4356,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -3004,7 +4364,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -3012,7 +4372,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -3020,7 +4380,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -3028,7 +4388,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -3036,7 +4396,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -3044,7 +4404,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -3052,7 +4412,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -3060,7 +4420,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -3068,7 +4428,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3094,13 +4454,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3111,7 +4471,7 @@
         <v>0.375</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3122,7 +4482,7 @@
         <v>0.72916666666666663</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated mapping table with new service messages
</commit_message>
<xml_diff>
--- a/data/mapping_tables.xlsx
+++ b/data/mapping_tables.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://maerskbroker-my.sharepoint.com/personal/kbo_maerskbroker_com/Documents/Documents/M scraper/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admkbo\Downloads\temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="637" documentId="8_{E82970A2-BBD4-4F32-BE27-31237F44A44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{68B89CBA-9803-41DF-9320-A846EF582A4E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{289020DD-1CCD-441B-B2F4-DAC6D01716C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2BAC1D2B-409C-4654-934D-3906D9663A7C}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="207">
   <si>
     <t>status_en</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>reason</t>
-  </si>
-  <si>
-    <t>Technical issues</t>
   </si>
   <si>
     <t>Maintenance</t>
@@ -607,6 +604,81 @@
   </si>
   <si>
     <t>Lukket frem til kl. 05:00 pga. sporarbejde. Metrobusser kører hvert 20. minut. Se afgangstider på rejseplanen.dk</t>
+  </si>
+  <si>
+    <t>M2: Passagerer til/fra Lufthavnen skal skifte tog på Christianshavn og Lergravsparken</t>
+  </si>
+  <si>
+    <t>I øjeblikket er der togskift på Lergravsparken</t>
+  </si>
+  <si>
+    <t>M1: Ingen togskift Ørestad-Vestamager pga. teknikere i sporet vi genoptager ca. kl. 15:48</t>
+  </si>
+  <si>
+    <t>Passagerer til og fra Vanløse skal skifte tog på Forum og Nørreport</t>
+  </si>
+  <si>
+    <t>ingen drift i øjeblikket. Vi genoptager drift kl. ca. 20:42</t>
+  </si>
+  <si>
+    <t>Alle passagerer mellem Vanløse - Lufthavnen skal skifte tog på Christianshavn. Dette skyldes et teknisk problem ved Amagerbro. Forvent længere rejsetid på strækningen mellem Christianshavn - Lufthavnen.</t>
+  </si>
+  <si>
+    <t>Alle passagerer mellem Vanløse - Lufthavnen skal skifte tog på Christianshavn.</t>
+  </si>
+  <si>
+    <t>Frem til kl. 05:00 erstatter metrobusser al togdrift på M1/M2. Busserne kører hvert 20. minut. Søg din rejse på rejseplanen.dk.</t>
+  </si>
+  <si>
+    <t>Alle passagerer som rejser til/fra Vanløse skal skifte tog på Frederiksberg. Det skyldes et tog med en teknisk fejl nær Lindevang. Forvent længere rejsetid mellem Vanløse - Frederiksberg. I tidsrummet 00:00-05:00 erstatter metrobusser al togdrift på M1/M2 pga. sporarbejde.</t>
+  </si>
+  <si>
+    <t>Passagerer til/fra Vanløse i begge spor skal skifte tog på Frederiksberg</t>
+  </si>
+  <si>
+    <t>Ingen togdrift ml. Vanløse og Frederiksberg pga. tog med teknisk problem ved Lindevang.</t>
+  </si>
+  <si>
+    <t>Forsinkelse ml. Christianshavn og Vestamager pga. langsomt kørende tog</t>
+  </si>
+  <si>
+    <t>Forsinkelser ml. Vanløse og Christianshavn pga. langsomt kørende tog</t>
+  </si>
+  <si>
+    <t>Forsinkelse ml. Nørreport-Vanløse pga. tog med teknisk problem på Nørreport</t>
+  </si>
+  <si>
+    <t>Christianshavn, Amagerbro, Lergravsparken, Øresund, Amager Strand, Femøren, Kastrup, CPH Lufthavn</t>
+  </si>
+  <si>
+    <t>Lergravsparken, Øresund, Amager Strand, Femøren, Kastrup, CPH Lufthavn</t>
+  </si>
+  <si>
+    <t>Ørestad, Vestamager</t>
+  </si>
+  <si>
+    <t>Nørreport, Forum, Frederiksberg, Fasanvej, Lindevang, Flintholm, Vanløse</t>
+  </si>
+  <si>
+    <t>Frederiksberg, Fasanvej, Lindevang, Flintholm, Vanløse</t>
+  </si>
+  <si>
+    <t>Islands Brygge, DR Byen, Sundby, Bella Center, Ørestad, Vestamager, Christianshavn</t>
+  </si>
+  <si>
+    <t>Technical issues with train(s)</t>
+  </si>
+  <si>
+    <t>Technical issues at a station</t>
+  </si>
+  <si>
+    <t>Christianshavn, Kongens Nytorv, Nørreport, Forum, Frederiksberg, Fasanvej, Lindevang, Flintholm, Vanløse</t>
+  </si>
+  <si>
+    <t>Technical issues (unspecified)</t>
+  </si>
+  <si>
+    <t>Technical issues between stations</t>
   </si>
 </sst>
 </file>
@@ -718,8 +790,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C314E41B-CB9C-4666-8112-1C776CCF8BCF}" name="Table2" displayName="Table2" ref="A1:I60" totalsRowShown="0">
-  <autoFilter ref="A1:I60" xr:uid="{C314E41B-CB9C-4666-8112-1C776CCF8BCF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C314E41B-CB9C-4666-8112-1C776CCF8BCF}" name="Table2" displayName="Table2" ref="A1:I74" totalsRowShown="0">
+  <autoFilter ref="A1:I74" xr:uid="{C314E41B-CB9C-4666-8112-1C776CCF8BCF}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A2B24526-B093-4F61-8528-751DBACD919A}" name="status_dk" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{AF80EE63-ECB6-42AC-8C94-7AE1E4203C14}" name="status_en" dataDxfId="9"/>
@@ -1079,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80E59BAE-EAED-4611-9ECD-D2146E9DBD95}">
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,7 +1172,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1121,7 +1193,7 @@
         <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
@@ -1153,12 +1225,12 @@
         <v>0</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>25</v>
@@ -1175,13 +1247,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -1200,7 +1272,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -1218,7 +1290,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1226,10 +1298,10 @@
         <v>24</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>29</v>
+        <v>202</v>
       </c>
       <c r="D6" s="4">
         <v>0</v>
@@ -1247,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -1255,10 +1327,10 @@
         <v>27</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>205</v>
       </c>
       <c r="D7" s="4">
         <v>0</v>
@@ -1276,18 +1348,18 @@
         <v>0</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="4">
         <v>0</v>
@@ -1308,129 +1380,129 @@
     </row>
     <row r="9" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4">
-        <v>1</v>
-      </c>
-      <c r="H9" s="4">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="G10" s="4">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0</v>
-      </c>
-      <c r="F11" s="4">
-        <v>1</v>
-      </c>
-      <c r="G11" s="4">
-        <v>1</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
-        <v>1</v>
-      </c>
-      <c r="G12" s="4">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4">
-        <v>0</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D13" s="4">
         <v>0</v>
@@ -1448,18 +1520,18 @@
         <v>0</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="C14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="4">
         <v>0</v>
@@ -1480,71 +1552,71 @@
     </row>
     <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0</v>
-      </c>
-      <c r="F15" s="4">
-        <v>0</v>
-      </c>
-      <c r="G15" s="4">
-        <v>1</v>
-      </c>
-      <c r="H15" s="4">
-        <v>0</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
-        <v>0</v>
-      </c>
-      <c r="G16" s="4">
-        <v>1</v>
-      </c>
-      <c r="H16" s="4">
-        <v>0</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="D17" s="4">
         <v>0</v>
@@ -1565,13 +1637,13 @@
     </row>
     <row r="18" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>29</v>
+        <v>203</v>
       </c>
       <c r="D18" s="4">
         <v>0</v>
@@ -1589,18 +1661,18 @@
         <v>1</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
@@ -1618,18 +1690,18 @@
         <v>1</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -1650,13 +1722,13 @@
     </row>
     <row r="21" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -1674,18 +1746,18 @@
         <v>0</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D22" s="4">
         <v>0</v>
@@ -1706,13 +1778,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D23" s="4">
         <v>0</v>
@@ -1733,13 +1805,13 @@
     </row>
     <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>29</v>
+        <v>205</v>
       </c>
       <c r="D24" s="4">
         <v>0</v>
@@ -1757,18 +1829,18 @@
         <v>0</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D25" s="4">
         <v>0</v>
@@ -1786,18 +1858,18 @@
         <v>1</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D26" s="4">
         <v>0</v>
@@ -1815,18 +1887,18 @@
         <v>1</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D27" s="4">
         <v>0</v>
@@ -1844,18 +1916,18 @@
         <v>1</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D28" s="4">
         <v>0</v>
@@ -1873,18 +1945,18 @@
         <v>0</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D29" s="4">
         <v>0</v>
@@ -1902,18 +1974,18 @@
         <v>0</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D30" s="4">
         <v>0</v>
@@ -1931,18 +2003,18 @@
         <v>0</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D31" s="4">
         <v>0</v>
@@ -1960,18 +2032,18 @@
         <v>0</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>29</v>
+        <v>203</v>
       </c>
       <c r="D32" s="4">
         <v>0</v>
@@ -1989,18 +2061,18 @@
         <v>0</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D33" s="4">
         <v>0</v>
@@ -2018,18 +2090,18 @@
         <v>0</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D34" s="4">
         <v>0</v>
@@ -2047,18 +2119,18 @@
         <v>0</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D35" s="4">
         <v>0</v>
@@ -2079,13 +2151,13 @@
     </row>
     <row r="36" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D36" s="4">
         <v>0</v>
@@ -2103,18 +2175,18 @@
         <v>0</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" s="4">
         <v>0</v>
@@ -2132,18 +2204,18 @@
         <v>0</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D38" s="4">
         <v>0</v>
@@ -2161,18 +2233,18 @@
         <v>0</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="144" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>29</v>
+        <v>203</v>
       </c>
       <c r="D39" s="4">
         <v>0</v>
@@ -2190,18 +2262,18 @@
         <v>1</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>29</v>
+        <v>202</v>
       </c>
       <c r="D40" s="4">
         <v>0</v>
@@ -2219,18 +2291,18 @@
         <v>0</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D41" s="4">
         <v>0</v>
@@ -2248,18 +2320,18 @@
         <v>0</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>29</v>
+        <v>203</v>
       </c>
       <c r="D42" s="4">
         <v>0</v>
@@ -2277,18 +2349,18 @@
         <v>0</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D43" s="4">
         <v>0</v>
@@ -2306,18 +2378,18 @@
         <v>0</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D44" s="4">
         <v>0</v>
@@ -2335,18 +2407,18 @@
         <v>0</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D45" s="4">
         <v>0</v>
@@ -2367,13 +2439,13 @@
     </row>
     <row r="46" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>29</v>
+        <v>205</v>
       </c>
       <c r="D46" s="4">
         <v>0</v>
@@ -2391,18 +2463,18 @@
         <v>0</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D47" s="4">
         <v>0</v>
@@ -2420,18 +2492,18 @@
         <v>1</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>29</v>
+        <v>203</v>
       </c>
       <c r="D48" s="4">
         <v>0</v>
@@ -2449,18 +2521,18 @@
         <v>0</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>29</v>
+        <v>203</v>
       </c>
       <c r="D49" s="4">
         <v>0</v>
@@ -2478,18 +2550,18 @@
         <v>0</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D50" s="4">
         <v>0</v>
@@ -2507,18 +2579,18 @@
         <v>0</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D51" s="4">
         <v>0</v>
@@ -2536,18 +2608,18 @@
         <v>1</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D52" s="4">
         <v>0</v>
@@ -2565,18 +2637,18 @@
         <v>1</v>
       </c>
       <c r="I52" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D53" s="4">
         <v>1</v>
@@ -2597,13 +2669,13 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D54" s="4">
         <v>1</v>
@@ -2624,13 +2696,13 @@
     </row>
     <row r="55" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D55" s="4">
         <v>0</v>
@@ -2648,18 +2720,18 @@
         <v>0</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56" s="4">
         <v>0</v>
@@ -2680,13 +2752,13 @@
     </row>
     <row r="57" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D57" s="4">
         <v>0</v>
@@ -2704,18 +2776,18 @@
         <v>0</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D58" s="4">
         <v>1</v>
@@ -2736,13 +2808,13 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D59" s="4">
         <v>0</v>
@@ -2760,18 +2832,18 @@
         <v>0</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D60" s="4">
         <v>1</v>
@@ -2789,6 +2861,412 @@
         <v>0</v>
       </c>
       <c r="I60" s="3"/>
+    </row>
+    <row r="61" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D61" s="4">
+        <v>0</v>
+      </c>
+      <c r="E61" s="4">
+        <v>1</v>
+      </c>
+      <c r="F61" s="4">
+        <v>0</v>
+      </c>
+      <c r="G61" s="4">
+        <v>0</v>
+      </c>
+      <c r="H61" s="4">
+        <v>1</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D62" s="4">
+        <v>0</v>
+      </c>
+      <c r="E62" s="4">
+        <v>1</v>
+      </c>
+      <c r="F62" s="4">
+        <v>0</v>
+      </c>
+      <c r="G62" s="4">
+        <v>0</v>
+      </c>
+      <c r="H62" s="4">
+        <v>1</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D63" s="4">
+        <v>0</v>
+      </c>
+      <c r="E63" s="4">
+        <v>0</v>
+      </c>
+      <c r="F63" s="4">
+        <v>1</v>
+      </c>
+      <c r="G63" s="4">
+        <v>0</v>
+      </c>
+      <c r="H63" s="4">
+        <v>0</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D64" s="4">
+        <v>0</v>
+      </c>
+      <c r="E64" s="4">
+        <v>1</v>
+      </c>
+      <c r="F64" s="4">
+        <v>0</v>
+      </c>
+      <c r="G64" s="4">
+        <v>0</v>
+      </c>
+      <c r="H64" s="4">
+        <v>1</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="4">
+        <v>0</v>
+      </c>
+      <c r="E65" s="4">
+        <v>0</v>
+      </c>
+      <c r="F65" s="4">
+        <v>1</v>
+      </c>
+      <c r="G65" s="4">
+        <v>0</v>
+      </c>
+      <c r="H65" s="4">
+        <v>0</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D66" s="4">
+        <v>0</v>
+      </c>
+      <c r="E66" s="4">
+        <v>1</v>
+      </c>
+      <c r="F66" s="4">
+        <v>0</v>
+      </c>
+      <c r="G66" s="4">
+        <v>0</v>
+      </c>
+      <c r="H66" s="4">
+        <v>1</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D67" s="4">
+        <v>0</v>
+      </c>
+      <c r="E67" s="4">
+        <v>1</v>
+      </c>
+      <c r="F67" s="4">
+        <v>0</v>
+      </c>
+      <c r="G67" s="4">
+        <v>0</v>
+      </c>
+      <c r="H67" s="4">
+        <v>1</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D68" s="4">
+        <v>1</v>
+      </c>
+      <c r="E68" s="4">
+        <v>0</v>
+      </c>
+      <c r="F68" s="4">
+        <v>0</v>
+      </c>
+      <c r="G68" s="4">
+        <v>0</v>
+      </c>
+      <c r="H68" s="4">
+        <v>0</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D69" s="4">
+        <v>0</v>
+      </c>
+      <c r="E69" s="4">
+        <v>1</v>
+      </c>
+      <c r="F69" s="4">
+        <v>0</v>
+      </c>
+      <c r="G69" s="4">
+        <v>0</v>
+      </c>
+      <c r="H69" s="4">
+        <v>1</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D70" s="4">
+        <v>0</v>
+      </c>
+      <c r="E70" s="4">
+        <v>1</v>
+      </c>
+      <c r="F70" s="4">
+        <v>0</v>
+      </c>
+      <c r="G70" s="4">
+        <v>0</v>
+      </c>
+      <c r="H70" s="4">
+        <v>1</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D71" s="4">
+        <v>0</v>
+      </c>
+      <c r="E71" s="4">
+        <v>0</v>
+      </c>
+      <c r="F71" s="4">
+        <v>1</v>
+      </c>
+      <c r="G71" s="4">
+        <v>0</v>
+      </c>
+      <c r="H71" s="4">
+        <v>0</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D72" s="4">
+        <v>0</v>
+      </c>
+      <c r="E72" s="4">
+        <v>1</v>
+      </c>
+      <c r="F72" s="4">
+        <v>0</v>
+      </c>
+      <c r="G72" s="4">
+        <v>0</v>
+      </c>
+      <c r="H72" s="4">
+        <v>0</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D73" s="4">
+        <v>0</v>
+      </c>
+      <c r="E73" s="4">
+        <v>1</v>
+      </c>
+      <c r="F73" s="4">
+        <v>0</v>
+      </c>
+      <c r="G73" s="4">
+        <v>0</v>
+      </c>
+      <c r="H73" s="4">
+        <v>0</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D74" s="4">
+        <v>0</v>
+      </c>
+      <c r="E74" s="4">
+        <v>1</v>
+      </c>
+      <c r="F74" s="4">
+        <v>0</v>
+      </c>
+      <c r="G74" s="4">
+        <v>0</v>
+      </c>
+      <c r="H74" s="4">
+        <v>0</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>199</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2818,59 +3296,59 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
         <v>112</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>113</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>115</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>116</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>117</v>
-      </c>
-      <c r="G1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" t="s">
         <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
       </c>
       <c r="D2">
         <v>2019</v>
       </c>
       <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>61</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
       </c>
       <c r="D3">
         <v>2007</v>
@@ -2882,18 +3360,18 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4">
         <v>2002</v>
@@ -2905,18 +3383,18 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5">
         <v>2002</v>
@@ -2928,18 +3406,18 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D6">
         <v>2003</v>
@@ -2951,18 +3429,18 @@
         <v>1</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7">
         <v>2003</v>
@@ -2974,18 +3452,18 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8">
         <v>2002</v>
@@ -2994,44 +3472,44 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9">
         <v>2019</v>
       </c>
       <c r="E9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
         <v>61</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10">
         <v>2003</v>
@@ -3043,18 +3521,18 @@
         <v>2</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D11">
         <v>2003</v>
@@ -3066,18 +3544,18 @@
         <v>2</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C12" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12">
         <v>2007</v>
@@ -3089,18 +3567,18 @@
         <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13">
         <v>2004</v>
@@ -3112,18 +3590,18 @@
         <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14">
         <v>2004</v>
@@ -3135,18 +3613,18 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D15">
         <v>2003</v>
@@ -3158,18 +3636,18 @@
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D16">
         <v>2003</v>
@@ -3181,18 +3659,18 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D17">
         <v>2003</v>
@@ -3201,21 +3679,21 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18">
         <v>2003</v>
@@ -3224,21 +3702,21 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D19">
         <v>2003</v>
@@ -3247,90 +3725,90 @@
         <v>3</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20">
         <v>2019</v>
       </c>
       <c r="E20" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>61</v>
-      </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D21">
         <v>2019</v>
       </c>
       <c r="E21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
         <v>61</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D22">
         <v>2019</v>
       </c>
       <c r="E22" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>61</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23">
         <v>2002</v>
@@ -3342,18 +3820,18 @@
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C24" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D24">
         <v>2007</v>
@@ -3365,64 +3843,64 @@
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D25">
         <v>2019</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D26">
         <v>2019</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D27">
         <v>2002</v>
@@ -3434,18 +3912,18 @@
         <v>1</v>
       </c>
       <c r="G27" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D28">
         <v>2002</v>
@@ -3457,18 +3935,18 @@
         <v>1</v>
       </c>
       <c r="G28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D29">
         <v>2002</v>
@@ -3480,18 +3958,18 @@
         <v>1</v>
       </c>
       <c r="G29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30">
         <v>2002</v>
@@ -3503,18 +3981,18 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D31">
         <v>2002</v>
@@ -3526,18 +4004,18 @@
         <v>1</v>
       </c>
       <c r="G31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32">
         <v>2003</v>
@@ -3549,18 +4027,18 @@
         <v>2</v>
       </c>
       <c r="G32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33">
         <v>2003</v>
@@ -3572,18 +4050,18 @@
         <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D34">
         <v>2007</v>
@@ -3595,133 +4073,133 @@
         <v>4</v>
       </c>
       <c r="G34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D35">
         <v>2019</v>
       </c>
       <c r="E35" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
         <v>61</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D36">
         <v>2019</v>
       </c>
       <c r="E36" t="s">
+        <v>60</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
         <v>61</v>
-      </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-      <c r="G36" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D37">
         <v>2020</v>
       </c>
       <c r="E37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F37">
         <v>2</v>
       </c>
       <c r="G37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D38">
         <v>2019</v>
       </c>
       <c r="E38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F38">
         <v>2</v>
       </c>
       <c r="G38" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B39" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D39">
         <v>2019</v>
       </c>
       <c r="E39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="G39" t="s">
         <v>61</v>
-      </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-      <c r="G39" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B40" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D40">
         <v>2002</v>
@@ -3733,18 +4211,18 @@
         <v>1</v>
       </c>
       <c r="G40" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D41">
         <v>2002</v>
@@ -3756,64 +4234,64 @@
         <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D42">
         <v>2019</v>
       </c>
       <c r="E42" t="s">
+        <v>60</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+      <c r="G42" t="s">
         <v>61</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D43">
         <v>2020</v>
       </c>
       <c r="E43" t="s">
+        <v>60</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43" t="s">
         <v>61</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D44">
         <v>2002</v>
@@ -3825,18 +4303,18 @@
         <v>3</v>
       </c>
       <c r="G44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D45">
         <v>2007</v>
@@ -3848,156 +4326,156 @@
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D46">
         <v>2019</v>
       </c>
       <c r="E46" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F46">
         <v>1</v>
       </c>
       <c r="G46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D47">
         <v>2019</v>
       </c>
       <c r="E47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F47">
         <v>1</v>
       </c>
       <c r="G47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D48">
         <v>2019</v>
       </c>
       <c r="E48" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48" t="s">
         <v>61</v>
-      </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C49" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D49">
         <v>2019</v>
       </c>
       <c r="E49" t="s">
+        <v>60</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+      <c r="G49" t="s">
         <v>61</v>
-      </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D50">
         <v>2019</v>
       </c>
       <c r="E50" t="s">
+        <v>60</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50" t="s">
         <v>61</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D51">
         <v>2019</v>
       </c>
       <c r="E51" t="s">
+        <v>60</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51" t="s">
         <v>61</v>
-      </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B52" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D52">
         <v>2002</v>
@@ -4009,41 +4487,41 @@
         <v>3</v>
       </c>
       <c r="G52" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B53" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D53">
         <v>2019</v>
       </c>
       <c r="E53" t="s">
+        <v>60</v>
+      </c>
+      <c r="F53">
+        <v>1</v>
+      </c>
+      <c r="G53" t="s">
         <v>61</v>
-      </c>
-      <c r="F53">
-        <v>1</v>
-      </c>
-      <c r="G53" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C54" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D54">
         <v>2003</v>
@@ -4055,18 +4533,18 @@
         <v>2</v>
       </c>
       <c r="G54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C55" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D55">
         <v>2003</v>
@@ -4078,18 +4556,18 @@
         <v>2</v>
       </c>
       <c r="G55" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C56" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D56">
         <v>2002</v>
@@ -4101,109 +4579,109 @@
         <v>3</v>
       </c>
       <c r="G56" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D57">
         <v>2019</v>
       </c>
       <c r="E57" t="s">
+        <v>60</v>
+      </c>
+      <c r="F57">
+        <v>1</v>
+      </c>
+      <c r="G57" t="s">
         <v>61</v>
-      </c>
-      <c r="F57">
-        <v>1</v>
-      </c>
-      <c r="G57" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D58">
         <v>2024</v>
       </c>
       <c r="G58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B59" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D59">
         <v>2024</v>
       </c>
       <c r="G59" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C60" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D60">
         <v>2024</v>
       </c>
       <c r="G60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D61">
         <v>2024</v>
       </c>
       <c r="G61" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B62" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D62">
         <v>2024</v>

</xml_diff>